<commit_message>
Thse changes are at 12:51 am
</commit_message>
<xml_diff>
--- a/Prayer.xlsx
+++ b/Prayer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3677" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3686" uniqueCount="74">
   <si>
     <t>Fajr</t>
   </si>
@@ -1348,6 +1348,21 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1357,15 +1372,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1373,12 +1379,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="9" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1664,8 +1664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC277"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A222" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="S234" sqref="S234"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A228" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="S240" sqref="S240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,7 +1726,7 @@
       </c>
       <c r="J1" s="68">
         <f ca="1">R1/(NOW()-DATE(2018,8,30))</f>
-        <v>19.676395296596667</v>
+        <v>19.629459949218209</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>15</v>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="R1" s="56">
         <f>SUM(R35,J35,C71,K71,S71,C108,K108,S108,C142,K142,S142,C177,K177,S177,C212,K212,S212,C247,K247,S247)</f>
-        <v>11258</v>
+        <v>11268</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>15</v>
@@ -1776,46 +1776,46 @@
       </c>
       <c r="Z1">
         <f ca="1">(20000000-SUM(J35,R35,C71,K71,S71,C108,K108,S108,C142,K142,S142,C177, K177, S177,C212,K212,S212)*1000)/J1/1000</f>
-        <v>508.01988114809632</v>
+        <v>509.23459055215199</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="40"/>
-      <c r="B2" s="213" t="s">
+      <c r="B2" s="218" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="213"/>
-      <c r="D2" s="213"/>
-      <c r="E2" s="213"/>
-      <c r="F2" s="213"/>
-      <c r="G2" s="213"/>
-      <c r="H2" s="213"/>
+      <c r="C2" s="218"/>
+      <c r="D2" s="218"/>
+      <c r="E2" s="218"/>
+      <c r="F2" s="218"/>
+      <c r="G2" s="218"/>
+      <c r="H2" s="218"/>
       <c r="I2" s="11"/>
-      <c r="J2" s="214" t="s">
+      <c r="J2" s="211" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="215"/>
-      <c r="L2" s="215"/>
-      <c r="M2" s="215"/>
-      <c r="N2" s="215"/>
-      <c r="O2" s="215"/>
-      <c r="P2" s="216"/>
+      <c r="K2" s="212"/>
+      <c r="L2" s="212"/>
+      <c r="M2" s="212"/>
+      <c r="N2" s="212"/>
+      <c r="O2" s="212"/>
+      <c r="P2" s="213"/>
       <c r="Q2" s="8"/>
-      <c r="R2" s="214" t="s">
+      <c r="R2" s="211" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="215"/>
-      <c r="T2" s="215"/>
-      <c r="U2" s="215"/>
-      <c r="V2" s="215"/>
-      <c r="W2" s="215"/>
-      <c r="X2" s="216"/>
+      <c r="S2" s="212"/>
+      <c r="T2" s="212"/>
+      <c r="U2" s="212"/>
+      <c r="V2" s="212"/>
+      <c r="W2" s="212"/>
+      <c r="X2" s="213"/>
       <c r="Y2" s="195" t="s">
         <v>55</v>
       </c>
       <c r="Z2" s="102">
         <f ca="1">NOW()+Z1</f>
-        <v>44422.177526402724</v>
+        <v>44425.269741246593</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
@@ -3095,7 +3095,7 @@
       <c r="X21" s="2"/>
       <c r="Y21" s="197">
         <f ca="1">NOW()-Y15</f>
-        <v>572.15764525462873</v>
+        <v>574.03515069444256</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
@@ -3165,7 +3165,7 @@
       <c r="X22" s="2"/>
       <c r="Y22" s="195">
         <f>R1/Y18</f>
-        <v>107.21904761904761</v>
+        <v>107.31428571428572</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -3894,21 +3894,21 @@
       <c r="P33" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="Q33" s="217" t="s">
+      <c r="Q33" s="219" t="s">
         <v>35</v>
       </c>
-      <c r="R33" s="218"/>
-      <c r="S33" s="218"/>
-      <c r="T33" s="218"/>
-      <c r="U33" s="218"/>
-      <c r="V33" s="218"/>
-      <c r="W33" s="218"/>
-      <c r="X33" s="219"/>
+      <c r="R33" s="220"/>
+      <c r="S33" s="220"/>
+      <c r="T33" s="220"/>
+      <c r="U33" s="220"/>
+      <c r="V33" s="220"/>
+      <c r="W33" s="220"/>
+      <c r="X33" s="221"/>
     </row>
     <row r="34" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="70">
         <f ca="1">TODAY()</f>
-        <v>43914</v>
+        <v>43916</v>
       </c>
       <c r="B34" s="18" t="s">
         <v>16</v>
@@ -4123,35 +4123,35 @@
     </row>
     <row r="38" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="70"/>
-      <c r="B38" s="214" t="s">
+      <c r="B38" s="211" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="215"/>
-      <c r="D38" s="215"/>
-      <c r="E38" s="215"/>
-      <c r="F38" s="215"/>
-      <c r="G38" s="215"/>
-      <c r="H38" s="216"/>
+      <c r="C38" s="212"/>
+      <c r="D38" s="212"/>
+      <c r="E38" s="212"/>
+      <c r="F38" s="212"/>
+      <c r="G38" s="212"/>
+      <c r="H38" s="213"/>
       <c r="I38" s="8"/>
-      <c r="J38" s="214" t="s">
+      <c r="J38" s="211" t="s">
         <v>13</v>
       </c>
-      <c r="K38" s="215"/>
-      <c r="L38" s="215"/>
-      <c r="M38" s="215"/>
-      <c r="N38" s="215"/>
-      <c r="O38" s="215"/>
-      <c r="P38" s="216"/>
+      <c r="K38" s="212"/>
+      <c r="L38" s="212"/>
+      <c r="M38" s="212"/>
+      <c r="N38" s="212"/>
+      <c r="O38" s="212"/>
+      <c r="P38" s="213"/>
       <c r="Q38" s="8"/>
-      <c r="R38" s="214" t="s">
+      <c r="R38" s="211" t="s">
         <v>14</v>
       </c>
-      <c r="S38" s="215"/>
-      <c r="T38" s="215"/>
-      <c r="U38" s="215"/>
-      <c r="V38" s="215"/>
-      <c r="W38" s="215"/>
-      <c r="X38" s="216"/>
+      <c r="S38" s="212"/>
+      <c r="T38" s="212"/>
+      <c r="U38" s="212"/>
+      <c r="V38" s="212"/>
+      <c r="W38" s="212"/>
+      <c r="X38" s="213"/>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -6400,13 +6400,13 @@
         <v>7</v>
       </c>
       <c r="I69" s="27"/>
-      <c r="J69" s="211"/>
-      <c r="K69" s="211"/>
-      <c r="L69" s="211"/>
-      <c r="M69" s="211"/>
-      <c r="N69" s="211"/>
-      <c r="O69" s="211"/>
-      <c r="P69" s="212"/>
+      <c r="J69" s="216"/>
+      <c r="K69" s="216"/>
+      <c r="L69" s="216"/>
+      <c r="M69" s="216"/>
+      <c r="N69" s="216"/>
+      <c r="O69" s="216"/>
+      <c r="P69" s="217"/>
       <c r="Q69" s="31" t="s">
         <v>29</v>
       </c>
@@ -6693,35 +6693,35 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" s="70"/>
-      <c r="B75" s="214" t="s">
+      <c r="B75" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="C75" s="215"/>
-      <c r="D75" s="215"/>
-      <c r="E75" s="215"/>
-      <c r="F75" s="215"/>
-      <c r="G75" s="215"/>
-      <c r="H75" s="216"/>
+      <c r="C75" s="212"/>
+      <c r="D75" s="212"/>
+      <c r="E75" s="212"/>
+      <c r="F75" s="212"/>
+      <c r="G75" s="212"/>
+      <c r="H75" s="213"/>
       <c r="I75" s="69"/>
-      <c r="J75" s="214" t="s">
+      <c r="J75" s="211" t="s">
         <v>43</v>
       </c>
-      <c r="K75" s="215"/>
-      <c r="L75" s="215"/>
-      <c r="M75" s="215"/>
-      <c r="N75" s="215"/>
-      <c r="O75" s="215"/>
-      <c r="P75" s="216"/>
+      <c r="K75" s="212"/>
+      <c r="L75" s="212"/>
+      <c r="M75" s="212"/>
+      <c r="N75" s="212"/>
+      <c r="O75" s="212"/>
+      <c r="P75" s="213"/>
       <c r="Q75" s="69"/>
-      <c r="R75" s="214" t="s">
+      <c r="R75" s="211" t="s">
         <v>44</v>
       </c>
-      <c r="S75" s="215"/>
-      <c r="T75" s="215"/>
-      <c r="U75" s="215"/>
-      <c r="V75" s="215"/>
-      <c r="W75" s="215"/>
-      <c r="X75" s="216"/>
+      <c r="S75" s="212"/>
+      <c r="T75" s="212"/>
+      <c r="U75" s="212"/>
+      <c r="V75" s="212"/>
+      <c r="W75" s="212"/>
+      <c r="X75" s="213"/>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
@@ -8897,13 +8897,13 @@
         <v>7</v>
       </c>
       <c r="I106" s="79"/>
-      <c r="J106" s="220"/>
-      <c r="K106" s="220"/>
-      <c r="L106" s="220"/>
-      <c r="M106" s="220"/>
-      <c r="N106" s="220"/>
-      <c r="O106" s="220"/>
-      <c r="P106" s="221"/>
+      <c r="J106" s="214"/>
+      <c r="K106" s="214"/>
+      <c r="L106" s="214"/>
+      <c r="M106" s="214"/>
+      <c r="N106" s="214"/>
+      <c r="O106" s="214"/>
+      <c r="P106" s="215"/>
       <c r="Q106" s="31" t="s">
         <v>28</v>
       </c>
@@ -9056,35 +9056,35 @@
     </row>
     <row r="109" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A109" s="70"/>
-      <c r="B109" s="214" t="s">
+      <c r="B109" s="211" t="s">
         <v>57</v>
       </c>
-      <c r="C109" s="215"/>
-      <c r="D109" s="215"/>
-      <c r="E109" s="215"/>
-      <c r="F109" s="215"/>
-      <c r="G109" s="215"/>
-      <c r="H109" s="216"/>
+      <c r="C109" s="212"/>
+      <c r="D109" s="212"/>
+      <c r="E109" s="212"/>
+      <c r="F109" s="212"/>
+      <c r="G109" s="212"/>
+      <c r="H109" s="213"/>
       <c r="I109" s="119"/>
-      <c r="J109" s="214" t="s">
+      <c r="J109" s="211" t="s">
         <v>58</v>
       </c>
-      <c r="K109" s="215"/>
-      <c r="L109" s="215"/>
-      <c r="M109" s="215"/>
-      <c r="N109" s="215"/>
-      <c r="O109" s="215"/>
-      <c r="P109" s="216"/>
+      <c r="K109" s="212"/>
+      <c r="L109" s="212"/>
+      <c r="M109" s="212"/>
+      <c r="N109" s="212"/>
+      <c r="O109" s="212"/>
+      <c r="P109" s="213"/>
       <c r="Q109" s="119"/>
-      <c r="R109" s="214" t="s">
+      <c r="R109" s="211" t="s">
         <v>59</v>
       </c>
-      <c r="S109" s="215"/>
-      <c r="T109" s="215"/>
-      <c r="U109" s="215"/>
-      <c r="V109" s="215"/>
-      <c r="W109" s="215"/>
-      <c r="X109" s="216"/>
+      <c r="S109" s="212"/>
+      <c r="T109" s="212"/>
+      <c r="U109" s="212"/>
+      <c r="V109" s="212"/>
+      <c r="W109" s="212"/>
+      <c r="X109" s="213"/>
     </row>
     <row r="110" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
@@ -10665,35 +10665,35 @@
     </row>
     <row r="143" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A143" s="70"/>
-      <c r="B143" s="214" t="s">
+      <c r="B143" s="211" t="s">
         <v>60</v>
       </c>
-      <c r="C143" s="215"/>
-      <c r="D143" s="215"/>
-      <c r="E143" s="215"/>
-      <c r="F143" s="215"/>
-      <c r="G143" s="215"/>
-      <c r="H143" s="216"/>
+      <c r="C143" s="212"/>
+      <c r="D143" s="212"/>
+      <c r="E143" s="212"/>
+      <c r="F143" s="212"/>
+      <c r="G143" s="212"/>
+      <c r="H143" s="213"/>
       <c r="I143" s="133"/>
-      <c r="J143" s="214" t="s">
+      <c r="J143" s="211" t="s">
         <v>61</v>
       </c>
-      <c r="K143" s="215"/>
-      <c r="L143" s="215"/>
-      <c r="M143" s="215"/>
-      <c r="N143" s="215"/>
-      <c r="O143" s="215"/>
-      <c r="P143" s="216"/>
+      <c r="K143" s="212"/>
+      <c r="L143" s="212"/>
+      <c r="M143" s="212"/>
+      <c r="N143" s="212"/>
+      <c r="O143" s="212"/>
+      <c r="P143" s="213"/>
       <c r="Q143" s="133"/>
-      <c r="R143" s="214" t="s">
+      <c r="R143" s="211" t="s">
         <v>62</v>
       </c>
-      <c r="S143" s="215"/>
-      <c r="T143" s="215"/>
-      <c r="U143" s="215"/>
-      <c r="V143" s="215"/>
-      <c r="W143" s="215"/>
-      <c r="X143" s="216"/>
+      <c r="S143" s="212"/>
+      <c r="T143" s="212"/>
+      <c r="U143" s="212"/>
+      <c r="V143" s="212"/>
+      <c r="W143" s="212"/>
+      <c r="X143" s="213"/>
     </row>
     <row r="144" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A144" s="70"/>
@@ -13175,35 +13175,35 @@
     </row>
     <row r="178" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A178" s="70"/>
-      <c r="B178" s="214" t="s">
+      <c r="B178" s="211" t="s">
         <v>65</v>
       </c>
-      <c r="C178" s="215"/>
-      <c r="D178" s="215"/>
-      <c r="E178" s="215"/>
-      <c r="F178" s="215"/>
-      <c r="G178" s="215"/>
-      <c r="H178" s="216"/>
+      <c r="C178" s="212"/>
+      <c r="D178" s="212"/>
+      <c r="E178" s="212"/>
+      <c r="F178" s="212"/>
+      <c r="G178" s="212"/>
+      <c r="H178" s="213"/>
       <c r="I178" s="170"/>
-      <c r="J178" s="214" t="s">
+      <c r="J178" s="211" t="s">
         <v>66</v>
       </c>
-      <c r="K178" s="215"/>
-      <c r="L178" s="215"/>
-      <c r="M178" s="215"/>
-      <c r="N178" s="215"/>
-      <c r="O178" s="215"/>
-      <c r="P178" s="216"/>
+      <c r="K178" s="212"/>
+      <c r="L178" s="212"/>
+      <c r="M178" s="212"/>
+      <c r="N178" s="212"/>
+      <c r="O178" s="212"/>
+      <c r="P178" s="213"/>
       <c r="Q178" s="170"/>
-      <c r="R178" s="214" t="s">
+      <c r="R178" s="211" t="s">
         <v>67</v>
       </c>
-      <c r="S178" s="215"/>
-      <c r="T178" s="215"/>
-      <c r="U178" s="215"/>
-      <c r="V178" s="215"/>
-      <c r="W178" s="215"/>
-      <c r="X178" s="216"/>
+      <c r="S178" s="212"/>
+      <c r="T178" s="212"/>
+      <c r="U178" s="212"/>
+      <c r="V178" s="212"/>
+      <c r="W178" s="212"/>
+      <c r="X178" s="213"/>
     </row>
     <row r="179" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A179" s="70"/>
@@ -14094,7 +14094,7 @@
       </c>
       <c r="Z190" s="177">
         <f ca="1">NOW()+Z188</f>
-        <v>43913.992532072203</v>
+        <v>43915.870037512017</v>
       </c>
     </row>
     <row r="191" spans="1:26" x14ac:dyDescent="0.25">
@@ -15706,35 +15706,35 @@
     </row>
     <row r="213" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A213" s="70"/>
-      <c r="B213" s="214" t="s">
+      <c r="B213" s="211" t="s">
         <v>68</v>
       </c>
-      <c r="C213" s="215"/>
-      <c r="D213" s="215"/>
-      <c r="E213" s="215"/>
-      <c r="F213" s="215"/>
-      <c r="G213" s="215"/>
-      <c r="H213" s="216"/>
+      <c r="C213" s="212"/>
+      <c r="D213" s="212"/>
+      <c r="E213" s="212"/>
+      <c r="F213" s="212"/>
+      <c r="G213" s="212"/>
+      <c r="H213" s="213"/>
       <c r="I213" s="191"/>
-      <c r="J213" s="214" t="s">
+      <c r="J213" s="211" t="s">
         <v>69</v>
       </c>
-      <c r="K213" s="215"/>
-      <c r="L213" s="215"/>
-      <c r="M213" s="215"/>
-      <c r="N213" s="215"/>
-      <c r="O213" s="215"/>
-      <c r="P213" s="216"/>
+      <c r="K213" s="212"/>
+      <c r="L213" s="212"/>
+      <c r="M213" s="212"/>
+      <c r="N213" s="212"/>
+      <c r="O213" s="212"/>
+      <c r="P213" s="213"/>
       <c r="Q213" s="191"/>
-      <c r="R213" s="214" t="s">
+      <c r="R213" s="211" t="s">
         <v>70</v>
       </c>
-      <c r="S213" s="215"/>
-      <c r="T213" s="215"/>
-      <c r="U213" s="215"/>
-      <c r="V213" s="215"/>
-      <c r="W213" s="215"/>
-      <c r="X213" s="216"/>
+      <c r="S213" s="212"/>
+      <c r="T213" s="212"/>
+      <c r="U213" s="212"/>
+      <c r="V213" s="212"/>
+      <c r="W213" s="212"/>
+      <c r="X213" s="213"/>
     </row>
     <row r="214" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A214" s="70"/>
@@ -17547,12 +17547,24 @@
       <c r="R238" s="10">
         <v>24</v>
       </c>
-      <c r="S238" s="125"/>
-      <c r="T238" s="185"/>
-      <c r="U238" s="185"/>
-      <c r="V238" s="186"/>
-      <c r="W238" s="97"/>
-      <c r="X238" s="97"/>
+      <c r="S238" s="125">
+        <v>10</v>
+      </c>
+      <c r="T238" s="185" t="s">
+        <v>8</v>
+      </c>
+      <c r="U238" s="185" t="s">
+        <v>8</v>
+      </c>
+      <c r="V238" s="186" t="s">
+        <v>7</v>
+      </c>
+      <c r="W238" s="97" t="s">
+        <v>7</v>
+      </c>
+      <c r="X238" s="97" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="239" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A239" s="16" t="s">
@@ -17610,10 +17622,18 @@
         <v>25</v>
       </c>
       <c r="S239" s="125"/>
-      <c r="T239" s="185"/>
-      <c r="U239" s="185"/>
-      <c r="V239" s="186"/>
-      <c r="W239" s="97"/>
+      <c r="T239" s="185" t="s">
+        <v>8</v>
+      </c>
+      <c r="U239" s="185" t="s">
+        <v>8</v>
+      </c>
+      <c r="V239" s="186" t="s">
+        <v>8</v>
+      </c>
+      <c r="W239" s="97" t="s">
+        <v>8</v>
+      </c>
       <c r="X239" s="97"/>
     </row>
     <row r="240" spans="1:24" x14ac:dyDescent="0.25">
@@ -18015,14 +18035,14 @@
       </c>
       <c r="U246" s="60">
         <f>COUNTIF(T215:X245,"T")</f>
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="V246" s="61" t="s">
         <v>39</v>
       </c>
       <c r="W246" s="60">
         <f>COUNTIF(T215:X245,"Q")</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X246" s="62"/>
     </row>
@@ -18073,21 +18093,21 @@
       <c r="P247" s="43"/>
       <c r="Q247" s="118">
         <f>S247/(31-COUNTIF(S215:S245,""))</f>
-        <v>11.913043478260869</v>
+        <v>11.833333333333334</v>
       </c>
       <c r="R247" s="63" t="s">
         <v>18</v>
       </c>
       <c r="S247" s="64">
         <f>SUM(S215:S245)</f>
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="T247" s="65" t="s">
         <v>37</v>
       </c>
       <c r="U247" s="136">
         <f>U246/(U246+W246)</f>
-        <v>0.48672566371681414</v>
+        <v>0.50819672131147542</v>
       </c>
       <c r="V247" s="63"/>
       <c r="W247" s="63"/>
@@ -18194,12 +18214,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B213:H213"/>
-    <mergeCell ref="J213:P213"/>
-    <mergeCell ref="R213:X213"/>
-    <mergeCell ref="B178:H178"/>
-    <mergeCell ref="J178:P178"/>
-    <mergeCell ref="R178:X178"/>
+    <mergeCell ref="J69:P69"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="R2:X2"/>
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="J38:P38"/>
+    <mergeCell ref="R38:X38"/>
+    <mergeCell ref="Q33:X33"/>
     <mergeCell ref="B75:H75"/>
     <mergeCell ref="J75:P75"/>
     <mergeCell ref="R75:X75"/>
@@ -18210,14 +18232,12 @@
     <mergeCell ref="B109:H109"/>
     <mergeCell ref="J109:P109"/>
     <mergeCell ref="R109:X109"/>
-    <mergeCell ref="J69:P69"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="R2:X2"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="J38:P38"/>
-    <mergeCell ref="R38:X38"/>
-    <mergeCell ref="Q33:X33"/>
+    <mergeCell ref="B213:H213"/>
+    <mergeCell ref="J213:P213"/>
+    <mergeCell ref="R213:X213"/>
+    <mergeCell ref="B178:H178"/>
+    <mergeCell ref="J178:P178"/>
+    <mergeCell ref="R178:X178"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>

</xml_diff>